<commit_message>
broken issue for opeing painting solved, name to ObjektID
</commit_message>
<xml_diff>
--- a/demo-data/PaintingZigeunerpaar.xlsx
+++ b/demo-data/PaintingZigeunerpaar.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">text</t>
   </si>
   <si>
-    <t xml:space="preserve">Objekt-ID</t>
+    <t xml:space="preserve">ObjektID</t>
   </si>
   <si>
     <t xml:space="preserve">Object1</t>
@@ -175,7 +175,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -205,6 +205,12 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Liberation Mono;Courier New;DejaVu Sans Mono;Lucida Sans Typewriter"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -248,7 +254,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -258,6 +264,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -458,7 +468,7 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -479,217 +489,217 @@
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="3" t="n">
+      <c r="B6" s="4" t="n">
         <v>1912</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="3"/>
+      <c r="B13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="3"/>
+      <c r="B15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="3"/>
+      <c r="B16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="3"/>
+      <c r="B17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="3"/>
+      <c r="B18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="3"/>
+      <c r="B19" s="4"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="3"/>
+      <c r="B20" s="4"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="4" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="4" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="4" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="3"/>
+      <c r="B24" s="4"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="3"/>
+      <c r="B25" s="4"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="3"/>
+      <c r="B26" s="4"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B27" s="3"/>
+      <c r="B27" s="4"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B28" s="3"/>
+      <c r="B28" s="4"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B29" s="3"/>
+      <c r="B29" s="4"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B30" s="3"/>
+      <c r="B30" s="4"/>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B31" s="3"/>
+      <c r="B31" s="4"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="4" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>